<commit_message>
Finalisation livrable 2 modélisation
</commit_message>
<xml_diff>
--- a/Livrable-2/Dictionnaire de données final.xlsx
+++ b/Livrable-2/Dictionnaire de données final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viacesifr-my.sharepoint.com/personal/anthony_schnepp_viacesi_fr/Documents/Bureau/Études One Drive/A2/Projets/Programmation orientée objet/Livrable 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{580B3F30-1DBD-4438-AD19-EBA9ADCE404F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{121C7E51-82C7-40DC-8A90-AA3E4F4737A6}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{580B3F30-1DBD-4438-AD19-EBA9ADCE404F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D8A61E-1C6D-499A-AE20-8953821CF7CC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB4EF615-54DA-4A8A-8E99-B0FF27B7371C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>N</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Nom_rue</t>
   </si>
   <si>
-    <t>Type_adresse</t>
-  </si>
-  <si>
     <t>Id_personne</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
   </si>
   <si>
     <t>Nom de rue</t>
-  </si>
-  <si>
-    <t>Type d'adresse (facturation ou livraison ou les deux)</t>
   </si>
   <si>
     <t>Prénom</t>
@@ -390,8 +384,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}" name="Tableau4234646" displayName="Tableau4234646" ref="A1:F34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F34" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}" name="Tableau4234646" displayName="Tableau4234646" ref="A1:F33" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F33" xr:uid="{D97F1EB4-EF69-4A77-9325-B5CC9874FEE7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A7585BCD-8D17-4F15-9C4B-7F44D4945DCF}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{9FC95855-C9FE-4C86-98B8-6295FE7C9BCA}" name="Type" dataDxfId="4"/>
@@ -701,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C508BB4-A982-4351-BEB9-D978C4430A2B}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -765,12 +759,12 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
@@ -781,7 +775,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -792,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -810,12 +804,12 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -831,7 +825,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -839,15 +833,17 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -855,17 +851,15 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -881,7 +875,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -889,15 +883,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>50</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -914,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -928,18 +920,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -947,21 +943,17 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3">
-        <v>30</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -975,51 +967,51 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="3">
-        <v>30</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,51 +1029,55 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3" t="s">
-        <v>1</v>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5" t="s">
-        <v>47</v>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3">
+        <v>30</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1089,49 +1085,47 @@
         <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C24" s="3">
-        <v>30</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="3">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1147,85 +1141,87 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="3" t="s">
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
+      <c r="C30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1236,30 +1232,12 @@
         <v>0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>